<commit_message>
Added new sections to CV
</commit_message>
<xml_diff>
--- a/vanlaar_vitae_data.xlsx
+++ b/vanlaar_vitae_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/triciavanlaar/Desktop/CSUStan/MiscWorkRelatedDocs/VanLaarCV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77D46A0-1BD2-5C4E-9D15-44D500EC7BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B7E792-5DD6-694E-AB1E-19F25C855218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="3340" windowWidth="26180" windowHeight="16260" activeTab="1" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="8380" yWindow="3340" windowWidth="26180" windowHeight="16260" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
@@ -63,6 +63,117 @@
     <t>The University of Texas at San Antonio</t>
   </si>
   <si>
+    <t>Major Advisor: J. Seshu, Ph.D.</t>
+  </si>
+  <si>
+    <t>MS Biology</t>
+  </si>
+  <si>
+    <t>University of the Pacific</t>
+  </si>
+  <si>
+    <t>San Antonio, TX</t>
+  </si>
+  <si>
+    <t>Stockton, CA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thesis Project: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>The behavior of Rad51D and XRCC2 in response to drug induced DNA damage and a continuing study of the fly Rad51 paralogs</t>
+    </r>
+  </si>
+  <si>
+    <t>Major Advisor: Lisa Wrischnik, Ph.D.</t>
+  </si>
+  <si>
+    <t>BS Biology</t>
+  </si>
+  <si>
+    <t>California State University, Stanislaus</t>
+  </si>
+  <si>
+    <t>Turlock, CA</t>
+  </si>
+  <si>
+    <t>Minor in Chemistry, Concentration in Genetics</t>
+  </si>
+  <si>
+    <t>Major Advisor: Jim Youngblom, Ph.D.</t>
+  </si>
+  <si>
+    <t>Assistant Professor of Microbial Genomics</t>
+  </si>
+  <si>
+    <t>Associate Professor of Microbiology</t>
+  </si>
+  <si>
+    <t>2022-Present</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>2015-2021</t>
+  </si>
+  <si>
+    <t>California State University, Fresno</t>
+  </si>
+  <si>
+    <t>Assistant Professor of Microbiology</t>
+  </si>
+  <si>
+    <t>Fresno, CA</t>
+  </si>
+  <si>
+    <t>Adjunct Instructor</t>
+  </si>
+  <si>
+    <t>St. Philip's College</t>
+  </si>
+  <si>
+    <t>2014-2015</t>
+  </si>
+  <si>
+    <t>NRC Post-Doctoral Research Fellow</t>
+  </si>
+  <si>
+    <t>US Army Institute for Surgical Research, Dental and Trauma Research Detachment</t>
+  </si>
+  <si>
+    <t>JBSA Fort Sam Houston, TX</t>
+  </si>
+  <si>
+    <t>2012-2015</t>
+  </si>
+  <si>
+    <t>Graduate Research and Teaching Assistant</t>
+  </si>
+  <si>
+    <t>2007-2012</t>
+  </si>
+  <si>
+    <t>2005-2007</t>
+  </si>
+  <si>
+    <t>Undergraduate Research Assistant</t>
+  </si>
+  <si>
+    <t>Endangered Species Recovery Program</t>
+  </si>
+  <si>
+    <t>2004-2005</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Dissertation Project: </t>
     </r>
@@ -89,118 +200,7 @@
     </r>
   </si>
   <si>
-    <t>Major Advisor: J. Seshu, Ph.D.</t>
-  </si>
-  <si>
-    <t>MS Biology</t>
-  </si>
-  <si>
-    <t>University of the Pacific</t>
-  </si>
-  <si>
-    <t>San Antonio, TX</t>
-  </si>
-  <si>
-    <t>Stockton, CA</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Thesis Project: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>The behavior of Rad51D and XRCC2 in response to drug induced DNA damage and a continuing study of the fly Rad51 paralogs</t>
-    </r>
-  </si>
-  <si>
-    <t>Major Advisor: Lisa Wrischnik, Ph.D.</t>
-  </si>
-  <si>
-    <t>BS Biology</t>
-  </si>
-  <si>
-    <t>California State University, Stanislaus</t>
-  </si>
-  <si>
-    <t>Turlock, CA</t>
-  </si>
-  <si>
-    <t>Minor in Chemistry, Concentration in Genetics</t>
-  </si>
-  <si>
     <t>Research Project: Speciation of Sylvilagus bachmani riparius</t>
-  </si>
-  <si>
-    <t>Major Advisor: Jim Youngblom, Ph.D.</t>
-  </si>
-  <si>
-    <t>Assistant Professor of Microbial Genomics</t>
-  </si>
-  <si>
-    <t>Associate Professor of Microbiology</t>
-  </si>
-  <si>
-    <t>2022-Present</t>
-  </si>
-  <si>
-    <t>2021-2022</t>
-  </si>
-  <si>
-    <t>2015-2021</t>
-  </si>
-  <si>
-    <t>California State University, Fresno</t>
-  </si>
-  <si>
-    <t>Assistant Professor of Microbiology</t>
-  </si>
-  <si>
-    <t>Fresno, CA</t>
-  </si>
-  <si>
-    <t>Adjunct Instructor</t>
-  </si>
-  <si>
-    <t>St. Philip's College</t>
-  </si>
-  <si>
-    <t>2014-2015</t>
-  </si>
-  <si>
-    <t>NRC Post-Doctoral Research Fellow</t>
-  </si>
-  <si>
-    <t>US Army Institute for Surgical Research, Dental and Trauma Research Detachment</t>
-  </si>
-  <si>
-    <t>JBSA Fort Sam Houston, TX</t>
-  </si>
-  <si>
-    <t>2012-2015</t>
-  </si>
-  <si>
-    <t>Graduate Research and Teaching Assistant</t>
-  </si>
-  <si>
-    <t>2007-2012</t>
-  </si>
-  <si>
-    <t>2005-2007</t>
-  </si>
-  <si>
-    <t>Undergraduate Research Assistant</t>
-  </si>
-  <si>
-    <t>Endangered Species Recovery Program</t>
-  </si>
-  <si>
-    <t>2004-2005</t>
   </si>
 </sst>
 </file>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4AE3D1-7C9F-C24D-A42B-F2C4925E72DD}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,10 +660,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -677,95 +677,95 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2007</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>2007</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>2005</v>
       </c>
       <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>2005</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>2005</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -778,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D85D00E-93F1-5A40-A255-93EE8D9FEFDC}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -800,114 +800,114 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>